<commit_message>
Added lab4 for cryptography and lab4 for flct
</commit_message>
<xml_diff>
--- a/cryptography/lab2/stats.xlsx
+++ b/cryptography/lab2/stats.xlsx
@@ -14,7 +14,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="22">
+  <si>
+    <t>1234567891011121314151617181920</t>
+  </si>
+  <si>
+    <t>9876543211011121314151617181920</t>
+  </si>
   <si>
     <t>85</t>
   </si>
@@ -139,39 +145,42 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$A$1:$A$10</c:f>
+              <c:f>Sheet1!$A$1:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>33</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>107</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>191</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>236</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>449</c:v>
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -188,39 +197,42 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$1:$B$10</c:f>
+              <c:f>Sheet1!$B$1:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>598</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>101</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>172</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>316</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>673</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>1021</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1141</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3223</c:v>
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>308</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -237,39 +249,42 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$1:$C$10</c:f>
+              <c:f>Sheet1!$C$1:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>1144247</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>219</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>232</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>501</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>475</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1463</c:v>
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>157</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -370,38 +385,41 @@
           <c:order val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$1:$D$10</c:f>
+              <c:f>Sheet1!$D$1:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>4</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>68</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>110</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>178</c:v>
                 </c:pt>
               </c:numCache>
@@ -838,7 +856,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -846,16 +864,16 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="B1">
-        <v>35</v>
+        <v>598</v>
       </c>
       <c r="C1">
-        <v>7</v>
+        <v>1144247</v>
       </c>
       <c r="D1">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -866,16 +884,16 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -886,16 +904,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="C3">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
@@ -906,16 +924,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>101</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -926,16 +944,16 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>172</v>
+        <v>14</v>
       </c>
       <c r="C5">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -946,16 +964,16 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>316</v>
+        <v>23</v>
       </c>
       <c r="C6">
-        <v>219</v>
+        <v>7</v>
       </c>
       <c r="D6">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -966,16 +984,16 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>107</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>673</v>
+        <v>35</v>
       </c>
       <c r="C7">
-        <v>232</v>
+        <v>23</v>
       </c>
       <c r="D7">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -986,16 +1004,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>191</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>1021</v>
+        <v>66</v>
       </c>
       <c r="C8">
-        <v>501</v>
+        <v>25</v>
       </c>
       <c r="D8">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -1006,16 +1024,16 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>236</v>
+        <v>19</v>
       </c>
       <c r="B9">
-        <v>1141</v>
+        <v>106</v>
       </c>
       <c r="C9">
-        <v>475</v>
+        <v>62</v>
       </c>
       <c r="D9">
-        <v>110</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
         <v>16</v>
@@ -1026,22 +1044,42 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>449</v>
+        <v>34</v>
       </c>
       <c r="B10">
-        <v>3223</v>
+        <v>167</v>
       </c>
       <c r="C10">
-        <v>1463</v>
+        <v>71</v>
       </c>
       <c r="D10">
-        <v>178</v>
+        <v>110</v>
       </c>
       <c r="E10" t="s">
         <v>18</v>
       </c>
       <c r="F10" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>58</v>
+      </c>
+      <c r="B11">
+        <v>308</v>
+      </c>
+      <c r="C11">
+        <v>157</v>
+      </c>
+      <c r="D11">
+        <v>178</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>